<commit_message>
starting the files for creating full data
</commit_message>
<xml_diff>
--- a/longitudinal ratings/exp set up/progress track guide.xlsx
+++ b/longitudinal ratings/exp set up/progress track guide.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="13940"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="12740" windowHeight="13940"/>
   </bookViews>
   <sheets>
     <sheet name="temp page for part no" sheetId="6" r:id="rId1"/>
@@ -30,49 +30,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>CHHS</author>
-  </authors>
-  <commentList>
-    <comment ref="A6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>CHHS:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>email</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>CHHS</author>
@@ -116,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="192">
   <si>
     <t>Person's Name</t>
   </si>
@@ -686,6 +643,12 @@
   </si>
   <si>
     <t>matched partno</t>
+  </si>
+  <si>
+    <t>entered overall ?</t>
+  </si>
+  <si>
+    <t>match group</t>
   </si>
 </sst>
 </file>
@@ -1891,16 +1854,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>187</v>
       </c>
@@ -1908,10 +1875,16 @@
         <v>188</v>
       </c>
       <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>66</v>
       </c>
@@ -1919,10 +1892,14 @@
         <v>555</v>
       </c>
       <c r="C2">
+        <f>B2+100</f>
+        <v>655</v>
+      </c>
+      <c r="D2">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>137</v>
       </c>
@@ -1930,10 +1907,14 @@
         <v>556</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C57" si="0">B3+100</f>
+        <v>656</v>
+      </c>
+      <c r="D3">
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
@@ -1941,10 +1922,14 @@
         <v>557</v>
       </c>
       <c r="C4">
+        <f t="shared" si="0"/>
+        <v>657</v>
+      </c>
+      <c r="D4">
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>104</v>
       </c>
@@ -1952,10 +1937,14 @@
         <v>558</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
+        <v>658</v>
+      </c>
+      <c r="D5">
         <v>336</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>162</v>
       </c>
@@ -1963,10 +1952,14 @@
         <v>559</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
+        <v>659</v>
+      </c>
+      <c r="D6">
         <v>337</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1974,10 +1967,14 @@
         <v>560</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
+        <v>660</v>
+      </c>
+      <c r="D7">
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>79</v>
       </c>
@@ -1985,10 +1982,14 @@
         <v>561</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>661</v>
+      </c>
+      <c r="D8">
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>66</v>
       </c>
@@ -1996,10 +1997,14 @@
         <v>562</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
+        <v>662</v>
+      </c>
+      <c r="D9">
         <v>340</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>150</v>
       </c>
@@ -2007,10 +2012,17 @@
         <v>563</v>
       </c>
       <c r="C10">
+        <f t="shared" si="0"/>
+        <v>663</v>
+      </c>
+      <c r="D10">
         <v>341</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>67</v>
       </c>
@@ -2018,10 +2030,14 @@
         <v>564</v>
       </c>
       <c r="C11">
+        <f t="shared" si="0"/>
+        <v>664</v>
+      </c>
+      <c r="D11">
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>133</v>
       </c>
@@ -2029,10 +2045,14 @@
         <v>565</v>
       </c>
       <c r="C12">
+        <f t="shared" si="0"/>
+        <v>665</v>
+      </c>
+      <c r="D12">
         <v>343</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>112</v>
       </c>
@@ -2040,10 +2060,14 @@
         <v>566</v>
       </c>
       <c r="C13">
+        <f t="shared" si="0"/>
+        <v>666</v>
+      </c>
+      <c r="D13">
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2051,10 +2075,14 @@
         <v>567</v>
       </c>
       <c r="C14">
+        <f t="shared" si="0"/>
+        <v>667</v>
+      </c>
+      <c r="D14">
         <v>345</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>85</v>
       </c>
@@ -2062,10 +2090,14 @@
         <v>568</v>
       </c>
       <c r="C15">
+        <f t="shared" si="0"/>
+        <v>668</v>
+      </c>
+      <c r="D15">
         <v>346</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>139</v>
       </c>
@@ -2073,10 +2105,14 @@
         <v>569</v>
       </c>
       <c r="C16">
+        <f t="shared" si="0"/>
+        <v>669</v>
+      </c>
+      <c r="D16">
         <v>347</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>54</v>
       </c>
@@ -2084,10 +2120,14 @@
         <v>570</v>
       </c>
       <c r="C17">
+        <f t="shared" si="0"/>
+        <v>670</v>
+      </c>
+      <c r="D17">
         <v>348</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>91</v>
       </c>
@@ -2095,10 +2135,14 @@
         <v>571</v>
       </c>
       <c r="C18">
+        <f t="shared" si="0"/>
+        <v>671</v>
+      </c>
+      <c r="D18">
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>102</v>
       </c>
@@ -2106,10 +2150,14 @@
         <v>572</v>
       </c>
       <c r="C19">
+        <f t="shared" si="0"/>
+        <v>672</v>
+      </c>
+      <c r="D19">
         <v>350</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>75</v>
       </c>
@@ -2117,10 +2165,14 @@
         <v>573</v>
       </c>
       <c r="C20">
+        <f t="shared" si="0"/>
+        <v>673</v>
+      </c>
+      <c r="D20">
         <v>351</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>77</v>
       </c>
@@ -2128,10 +2180,14 @@
         <v>574</v>
       </c>
       <c r="C21">
+        <f t="shared" si="0"/>
+        <v>674</v>
+      </c>
+      <c r="D21">
         <v>352</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -2139,10 +2195,14 @@
         <v>575</v>
       </c>
       <c r="C22">
+        <f t="shared" si="0"/>
+        <v>675</v>
+      </c>
+      <c r="D22">
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
@@ -2150,10 +2210,14 @@
         <v>576</v>
       </c>
       <c r="C23">
+        <f t="shared" si="0"/>
+        <v>676</v>
+      </c>
+      <c r="D23">
         <v>354</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
@@ -2161,10 +2225,14 @@
         <v>577</v>
       </c>
       <c r="C24">
+        <f t="shared" si="0"/>
+        <v>677</v>
+      </c>
+      <c r="D24">
         <v>355</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>100</v>
       </c>
@@ -2172,10 +2240,14 @@
         <v>578</v>
       </c>
       <c r="C25">
+        <f t="shared" si="0"/>
+        <v>678</v>
+      </c>
+      <c r="D25">
         <v>356</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>110</v>
       </c>
@@ -2183,10 +2255,14 @@
         <v>579</v>
       </c>
       <c r="C26">
+        <f t="shared" si="0"/>
+        <v>679</v>
+      </c>
+      <c r="D26">
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>82</v>
       </c>
@@ -2194,10 +2270,14 @@
         <v>580</v>
       </c>
       <c r="C27">
+        <f t="shared" si="0"/>
+        <v>680</v>
+      </c>
+      <c r="D27">
         <v>358</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2205,10 +2285,14 @@
         <v>581</v>
       </c>
       <c r="C28">
+        <f t="shared" si="0"/>
+        <v>681</v>
+      </c>
+      <c r="D28">
         <v>359</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>116</v>
       </c>
@@ -2216,10 +2300,14 @@
         <v>582</v>
       </c>
       <c r="C29">
+        <f t="shared" si="0"/>
+        <v>682</v>
+      </c>
+      <c r="D29">
         <v>360</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>46</v>
       </c>
@@ -2227,10 +2315,14 @@
         <v>583</v>
       </c>
       <c r="C30">
+        <f t="shared" si="0"/>
+        <v>683</v>
+      </c>
+      <c r="D30">
         <v>361</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
         <v>159</v>
       </c>
@@ -2238,10 +2330,14 @@
         <v>584</v>
       </c>
       <c r="C31">
+        <f t="shared" si="0"/>
+        <v>684</v>
+      </c>
+      <c r="D31">
         <v>362</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>157</v>
       </c>
@@ -2249,10 +2345,14 @@
         <v>585</v>
       </c>
       <c r="C32">
+        <f t="shared" si="0"/>
+        <v>685</v>
+      </c>
+      <c r="D32">
         <v>363</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
         <v>19</v>
       </c>
@@ -2260,10 +2360,14 @@
         <v>586</v>
       </c>
       <c r="C33">
+        <f t="shared" si="0"/>
+        <v>686</v>
+      </c>
+      <c r="D33">
         <v>364</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>95</v>
       </c>
@@ -2271,10 +2375,14 @@
         <v>587</v>
       </c>
       <c r="C34">
+        <f t="shared" si="0"/>
+        <v>687</v>
+      </c>
+      <c r="D34">
         <v>365</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>52</v>
       </c>
@@ -2282,10 +2390,14 @@
         <v>588</v>
       </c>
       <c r="C35">
+        <f t="shared" si="0"/>
+        <v>688</v>
+      </c>
+      <c r="D35">
         <v>366</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>119</v>
       </c>
@@ -2293,10 +2405,14 @@
         <v>589</v>
       </c>
       <c r="C36">
+        <f t="shared" si="0"/>
+        <v>689</v>
+      </c>
+      <c r="D36">
         <v>367</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>163</v>
       </c>
@@ -2304,10 +2420,14 @@
         <v>590</v>
       </c>
       <c r="C37">
+        <f t="shared" si="0"/>
+        <v>690</v>
+      </c>
+      <c r="D37">
         <v>368</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>48</v>
       </c>
@@ -2315,10 +2435,14 @@
         <v>591</v>
       </c>
       <c r="C38">
+        <f t="shared" si="0"/>
+        <v>691</v>
+      </c>
+      <c r="D38">
         <v>369</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>98</v>
       </c>
@@ -2326,10 +2450,14 @@
         <v>592</v>
       </c>
       <c r="C39">
+        <f t="shared" si="0"/>
+        <v>692</v>
+      </c>
+      <c r="D39">
         <v>370</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>146</v>
       </c>
@@ -2337,10 +2465,14 @@
         <v>593</v>
       </c>
       <c r="C40">
+        <f t="shared" si="0"/>
+        <v>693</v>
+      </c>
+      <c r="D40">
         <v>371</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="24" t="s">
         <v>153</v>
       </c>
@@ -2348,10 +2480,14 @@
         <v>594</v>
       </c>
       <c r="C41">
+        <f t="shared" si="0"/>
+        <v>694</v>
+      </c>
+      <c r="D41">
         <v>372</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
         <v>108</v>
       </c>
@@ -2359,10 +2495,14 @@
         <v>595</v>
       </c>
       <c r="C42">
+        <f t="shared" si="0"/>
+        <v>695</v>
+      </c>
+      <c r="D42">
         <v>373</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>21</v>
       </c>
@@ -2370,10 +2510,14 @@
         <v>596</v>
       </c>
       <c r="C43">
+        <f t="shared" si="0"/>
+        <v>696</v>
+      </c>
+      <c r="D43">
         <v>374</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>94</v>
       </c>
@@ -2381,10 +2525,14 @@
         <v>597</v>
       </c>
       <c r="C44">
+        <f t="shared" si="0"/>
+        <v>697</v>
+      </c>
+      <c r="D44">
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>155</v>
       </c>
@@ -2392,10 +2540,14 @@
         <v>598</v>
       </c>
       <c r="C45">
+        <f t="shared" si="0"/>
+        <v>698</v>
+      </c>
+      <c r="D45">
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>170</v>
       </c>
@@ -2403,10 +2555,14 @@
         <v>599</v>
       </c>
       <c r="C46">
+        <f t="shared" si="0"/>
+        <v>699</v>
+      </c>
+      <c r="D46">
         <v>377</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>136</v>
       </c>
@@ -2414,10 +2570,14 @@
         <v>600</v>
       </c>
       <c r="C47">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="D47">
         <v>378</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>131</v>
       </c>
@@ -2425,10 +2585,14 @@
         <v>601</v>
       </c>
       <c r="C48">
+        <f t="shared" si="0"/>
+        <v>701</v>
+      </c>
+      <c r="D48">
         <v>379</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>73</v>
       </c>
@@ -2436,10 +2600,14 @@
         <v>602</v>
       </c>
       <c r="C49">
+        <f t="shared" si="0"/>
+        <v>702</v>
+      </c>
+      <c r="D49">
         <v>380</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
         <v>114</v>
       </c>
@@ -2447,10 +2615,14 @@
         <v>603</v>
       </c>
       <c r="C50">
+        <f t="shared" si="0"/>
+        <v>703</v>
+      </c>
+      <c r="D50">
         <v>381</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
         <v>106</v>
       </c>
@@ -2458,10 +2630,14 @@
         <v>604</v>
       </c>
       <c r="C51">
+        <f t="shared" si="0"/>
+        <v>704</v>
+      </c>
+      <c r="D51">
         <v>382</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>118</v>
       </c>
@@ -2469,10 +2645,14 @@
         <v>605</v>
       </c>
       <c r="C52">
+        <f t="shared" si="0"/>
+        <v>705</v>
+      </c>
+      <c r="D52">
         <v>383</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>69</v>
       </c>
@@ -2480,10 +2660,14 @@
         <v>606</v>
       </c>
       <c r="C53">
+        <f t="shared" si="0"/>
+        <v>706</v>
+      </c>
+      <c r="D53">
         <v>384</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>35</v>
       </c>
@@ -2491,10 +2675,14 @@
         <v>607</v>
       </c>
       <c r="C54">
+        <f t="shared" si="0"/>
+        <v>707</v>
+      </c>
+      <c r="D54">
         <v>385</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
         <v>149</v>
       </c>
@@ -2502,10 +2690,17 @@
         <v>608</v>
       </c>
       <c r="C55">
+        <f t="shared" si="0"/>
+        <v>708</v>
+      </c>
+      <c r="D55">
         <v>386</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
@@ -2513,10 +2708,14 @@
         <v>609</v>
       </c>
       <c r="C56">
+        <f t="shared" si="0"/>
+        <v>709</v>
+      </c>
+      <c r="D56">
         <v>387</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>71</v>
       </c>
@@ -2524,6 +2723,10 @@
         <v>610</v>
       </c>
       <c r="C57">
+        <f t="shared" si="0"/>
+        <v>710</v>
+      </c>
+      <c r="D57">
         <v>388</v>
       </c>
     </row>
@@ -2532,7 +2735,6 @@
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>